<commit_message>
Adressed review and updated excel sheets
</commit_message>
<xml_diff>
--- a/tests/fixtures/orderforms/1508.27.balsamic.xlsx
+++ b/tests/fixtures/orderforms/1508.27.balsamic.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vincent.janvid/dev/cg/tests/fixtures/orderforms/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C4A6724-9214-7C4F-B1DF-F19335359DFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31D24F99-2FEC-AF47-993E-4A014FB858BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="-8280" windowWidth="51080" windowHeight="26280" tabRatio="993" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28900" yWindow="-8280" windowWidth="51080" windowHeight="26280" tabRatio="993" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="information" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1338" uniqueCount="707">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1301" uniqueCount="712">
   <si>
     <t>https://clinical.scilifelab.se/</t>
   </si>
@@ -3085,6 +3085,21 @@
   <si>
     <t>Reference Genome</t>
   </si>
+  <si>
+    <t>Fastq + Scout</t>
+  </si>
+  <si>
+    <t>cust902</t>
+  </si>
+  <si>
+    <t>cust903</t>
+  </si>
+  <si>
+    <t>cust904</t>
+  </si>
+  <si>
+    <t>cust905</t>
+  </si>
 </sst>
 </file>
 
@@ -4255,6 +4270,7 @@
     </xf>
     <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -4288,7 +4304,6 @@
     <xf numFmtId="49" fontId="3" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="25">
     <cellStyle name="Excel Built-in Normal" xfId="24" xr:uid="{3FDE16F9-6A75-4E47-AB2C-EADD63120127}"/>
@@ -5382,8 +5397,8 @@
   </sheetPr>
   <dimension ref="A1:AMO395"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A35" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="G49" sqref="G49"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" outlineLevelRow="1" x14ac:dyDescent="0.15"/>
@@ -11690,34 +11705,34 @@
       <c r="AL8" s="33"/>
     </row>
     <row r="9" spans="1:1028" s="39" customFormat="1" ht="22" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="177" t="s">
+      <c r="A9" s="178" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="178"/>
-      <c r="C9" s="178"/>
-      <c r="D9" s="178"/>
-      <c r="E9" s="178"/>
-      <c r="F9" s="178"/>
-      <c r="G9" s="178"/>
-      <c r="H9" s="178"/>
-      <c r="I9" s="178"/>
-      <c r="J9" s="178"/>
-      <c r="K9" s="178"/>
-      <c r="L9" s="178"/>
-      <c r="M9" s="178"/>
-      <c r="N9" s="179"/>
+      <c r="B9" s="179"/>
+      <c r="C9" s="179"/>
+      <c r="D9" s="179"/>
+      <c r="E9" s="179"/>
+      <c r="F9" s="179"/>
+      <c r="G9" s="179"/>
+      <c r="H9" s="179"/>
+      <c r="I9" s="179"/>
+      <c r="J9" s="179"/>
+      <c r="K9" s="179"/>
+      <c r="L9" s="179"/>
+      <c r="M9" s="179"/>
+      <c r="N9" s="180"/>
       <c r="O9" s="35"/>
-      <c r="P9" s="181" t="s">
+      <c r="P9" s="182" t="s">
         <v>13</v>
       </c>
-      <c r="Q9" s="181"/>
+      <c r="Q9" s="182"/>
       <c r="R9" s="116"/>
-      <c r="S9" s="182" t="s">
+      <c r="S9" s="183" t="s">
         <v>14</v>
       </c>
-      <c r="T9" s="183"/>
-      <c r="U9" s="183"/>
-      <c r="V9" s="184"/>
+      <c r="T9" s="184"/>
+      <c r="U9" s="184"/>
+      <c r="V9" s="185"/>
       <c r="W9" s="36"/>
       <c r="X9" s="37" t="s">
         <v>15</v>
@@ -11727,23 +11742,23 @@
         <v>16</v>
       </c>
       <c r="AA9" s="38"/>
-      <c r="AB9" s="180" t="s">
+      <c r="AB9" s="181" t="s">
         <v>17</v>
       </c>
-      <c r="AC9" s="180"/>
-      <c r="AD9" s="180"/>
+      <c r="AC9" s="181"/>
+      <c r="AD9" s="181"/>
       <c r="AE9" s="36"/>
       <c r="AF9" s="167" t="s">
         <v>704</v>
       </c>
       <c r="AG9" s="168"/>
-      <c r="AH9" s="185" t="s">
+      <c r="AH9" s="186" t="s">
         <v>6</v>
       </c>
-      <c r="AI9" s="186"/>
-      <c r="AJ9" s="186"/>
-      <c r="AK9" s="186"/>
-      <c r="AL9" s="187"/>
+      <c r="AI9" s="187"/>
+      <c r="AJ9" s="187"/>
+      <c r="AK9" s="187"/>
+      <c r="AL9" s="188"/>
     </row>
     <row r="10" spans="1:1028" ht="13" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="40" t="s">
@@ -13145,9 +13160,7 @@
         <v>83</v>
       </c>
       <c r="AE15" s="55"/>
-      <c r="AF15" s="102" t="s">
-        <v>701</v>
-      </c>
+      <c r="AF15" s="102"/>
       <c r="AG15" s="173"/>
       <c r="AH15" s="96" t="s">
         <v>533</v>
@@ -14223,9 +14236,7 @@
         <v>95</v>
       </c>
       <c r="AE16" s="55"/>
-      <c r="AF16" s="102" t="s">
-        <v>701</v>
-      </c>
+      <c r="AF16" s="102"/>
       <c r="AG16" s="173"/>
       <c r="AH16" s="96" t="s">
         <v>534</v>
@@ -15291,9 +15302,7 @@
       <c r="AC17" s="103"/>
       <c r="AD17" s="102"/>
       <c r="AE17" s="55"/>
-      <c r="AF17" s="102" t="s">
-        <v>701</v>
-      </c>
+      <c r="AF17" s="102"/>
       <c r="AG17" s="173"/>
       <c r="AH17" s="96"/>
       <c r="AI17" s="99"/>
@@ -16357,9 +16366,7 @@
       <c r="AC18" s="103"/>
       <c r="AD18" s="102"/>
       <c r="AE18" s="55"/>
-      <c r="AF18" s="102" t="s">
-        <v>701</v>
-      </c>
+      <c r="AF18" s="102"/>
       <c r="AG18" s="173"/>
       <c r="AH18" s="96"/>
       <c r="AI18" s="99"/>
@@ -17423,9 +17430,7 @@
       <c r="AC19" s="103"/>
       <c r="AD19" s="102"/>
       <c r="AE19" s="55"/>
-      <c r="AF19" s="102" t="s">
-        <v>701</v>
-      </c>
+      <c r="AF19" s="102"/>
       <c r="AG19" s="173"/>
       <c r="AH19" s="96"/>
       <c r="AI19" s="99"/>
@@ -18489,9 +18494,7 @@
       <c r="AC20" s="103"/>
       <c r="AD20" s="102"/>
       <c r="AE20" s="55"/>
-      <c r="AF20" s="102" t="s">
-        <v>701</v>
-      </c>
+      <c r="AF20" s="102"/>
       <c r="AG20" s="173"/>
       <c r="AH20" s="96"/>
       <c r="AI20" s="99"/>
@@ -19555,9 +19558,7 @@
       <c r="AC21" s="103"/>
       <c r="AD21" s="102"/>
       <c r="AE21" s="55"/>
-      <c r="AF21" s="102" t="s">
-        <v>701</v>
-      </c>
+      <c r="AF21" s="102"/>
       <c r="AG21" s="173"/>
       <c r="AH21" s="96"/>
       <c r="AI21" s="99"/>
@@ -20621,9 +20622,7 @@
       <c r="AC22" s="103"/>
       <c r="AD22" s="102"/>
       <c r="AE22" s="55"/>
-      <c r="AF22" s="102" t="s">
-        <v>701</v>
-      </c>
+      <c r="AF22" s="102"/>
       <c r="AG22" s="173"/>
       <c r="AH22" s="96"/>
       <c r="AI22" s="99"/>
@@ -21687,9 +21686,7 @@
       <c r="AC23" s="103"/>
       <c r="AD23" s="102"/>
       <c r="AE23" s="55"/>
-      <c r="AF23" s="102" t="s">
-        <v>701</v>
-      </c>
+      <c r="AF23" s="102"/>
       <c r="AG23" s="173"/>
       <c r="AH23" s="96"/>
       <c r="AI23" s="99"/>
@@ -22753,9 +22750,7 @@
       <c r="AC24" s="103"/>
       <c r="AD24" s="102"/>
       <c r="AE24" s="55"/>
-      <c r="AF24" s="102" t="s">
-        <v>701</v>
-      </c>
+      <c r="AF24" s="102"/>
       <c r="AG24" s="173"/>
       <c r="AH24" s="96"/>
       <c r="AI24" s="99"/>
@@ -23819,9 +23814,7 @@
       <c r="AC25" s="103"/>
       <c r="AD25" s="102"/>
       <c r="AE25" s="55"/>
-      <c r="AF25" s="102" t="s">
-        <v>701</v>
-      </c>
+      <c r="AF25" s="102"/>
       <c r="AG25" s="173"/>
       <c r="AH25" s="96"/>
       <c r="AI25" s="99"/>
@@ -24885,9 +24878,7 @@
       <c r="AC26" s="103"/>
       <c r="AD26" s="102"/>
       <c r="AE26" s="55"/>
-      <c r="AF26" s="102" t="s">
-        <v>701</v>
-      </c>
+      <c r="AF26" s="102"/>
       <c r="AG26" s="173"/>
       <c r="AH26" s="96"/>
       <c r="AI26" s="99"/>
@@ -25951,9 +25942,7 @@
       <c r="AC27" s="103"/>
       <c r="AD27" s="102"/>
       <c r="AE27" s="55"/>
-      <c r="AF27" s="102" t="s">
-        <v>701</v>
-      </c>
+      <c r="AF27" s="102"/>
       <c r="AG27" s="173"/>
       <c r="AH27" s="96"/>
       <c r="AI27" s="99"/>
@@ -26027,9 +26016,7 @@
       <c r="AC28" s="103"/>
       <c r="AD28" s="102"/>
       <c r="AE28" s="55"/>
-      <c r="AF28" s="102" t="s">
-        <v>701</v>
-      </c>
+      <c r="AF28" s="102"/>
       <c r="AG28" s="173"/>
       <c r="AH28" s="96"/>
       <c r="AI28" s="99"/>
@@ -27093,9 +27080,7 @@
       <c r="AC29" s="103"/>
       <c r="AD29" s="102"/>
       <c r="AE29" s="55"/>
-      <c r="AF29" s="102" t="s">
-        <v>701</v>
-      </c>
+      <c r="AF29" s="102"/>
       <c r="AG29" s="173"/>
       <c r="AH29" s="96"/>
       <c r="AI29" s="99"/>
@@ -28159,9 +28144,7 @@
       <c r="AC30" s="103"/>
       <c r="AD30" s="102"/>
       <c r="AE30" s="55"/>
-      <c r="AF30" s="102" t="s">
-        <v>701</v>
-      </c>
+      <c r="AF30" s="102"/>
       <c r="AG30" s="173"/>
       <c r="AH30" s="96"/>
       <c r="AI30" s="99"/>
@@ -29225,9 +29208,7 @@
       <c r="AC31" s="103"/>
       <c r="AD31" s="102"/>
       <c r="AE31" s="55"/>
-      <c r="AF31" s="102" t="s">
-        <v>701</v>
-      </c>
+      <c r="AF31" s="102"/>
       <c r="AG31" s="173"/>
       <c r="AH31" s="96"/>
       <c r="AI31" s="99"/>
@@ -30291,9 +30272,7 @@
       <c r="AC32" s="103"/>
       <c r="AD32" s="102"/>
       <c r="AE32" s="55"/>
-      <c r="AF32" s="102" t="s">
-        <v>701</v>
-      </c>
+      <c r="AF32" s="102"/>
       <c r="AG32" s="173"/>
       <c r="AH32" s="96"/>
       <c r="AI32" s="99"/>
@@ -31357,9 +31336,7 @@
       <c r="AC33" s="103"/>
       <c r="AD33" s="102"/>
       <c r="AE33" s="55"/>
-      <c r="AF33" s="102" t="s">
-        <v>701</v>
-      </c>
+      <c r="AF33" s="102"/>
       <c r="AG33" s="173"/>
       <c r="AH33" s="96"/>
       <c r="AI33" s="99"/>
@@ -32423,9 +32400,7 @@
       <c r="AC34" s="103"/>
       <c r="AD34" s="102"/>
       <c r="AE34" s="55"/>
-      <c r="AF34" s="102" t="s">
-        <v>701</v>
-      </c>
+      <c r="AF34" s="102"/>
       <c r="AG34" s="173"/>
       <c r="AH34" s="96"/>
       <c r="AI34" s="99"/>
@@ -33489,9 +33464,7 @@
       <c r="AC35" s="103"/>
       <c r="AD35" s="102"/>
       <c r="AE35" s="55"/>
-      <c r="AF35" s="102" t="s">
-        <v>701</v>
-      </c>
+      <c r="AF35" s="102"/>
       <c r="AG35" s="173"/>
       <c r="AH35" s="96"/>
       <c r="AI35" s="99"/>
@@ -34555,9 +34528,7 @@
       <c r="AC36" s="103"/>
       <c r="AD36" s="102"/>
       <c r="AE36" s="55"/>
-      <c r="AF36" s="102" t="s">
-        <v>701</v>
-      </c>
+      <c r="AF36" s="102"/>
       <c r="AG36" s="173"/>
       <c r="AH36" s="96"/>
       <c r="AI36" s="99"/>
@@ -34631,9 +34602,7 @@
       <c r="AC37" s="103"/>
       <c r="AD37" s="102"/>
       <c r="AE37" s="55"/>
-      <c r="AF37" s="102" t="s">
-        <v>701</v>
-      </c>
+      <c r="AF37" s="102"/>
       <c r="AG37" s="173"/>
       <c r="AH37" s="96"/>
       <c r="AI37" s="99"/>
@@ -34709,9 +34678,7 @@
       <c r="AC38" s="103"/>
       <c r="AD38" s="102"/>
       <c r="AE38" s="55"/>
-      <c r="AF38" s="102" t="s">
-        <v>701</v>
-      </c>
+      <c r="AF38" s="102"/>
       <c r="AG38" s="173"/>
       <c r="AH38" s="96"/>
       <c r="AI38" s="99"/>
@@ -34787,9 +34754,7 @@
       <c r="AC39" s="103"/>
       <c r="AD39" s="102"/>
       <c r="AE39" s="55"/>
-      <c r="AF39" s="102" t="s">
-        <v>701</v>
-      </c>
+      <c r="AF39" s="102"/>
       <c r="AG39" s="173"/>
       <c r="AH39" s="96"/>
       <c r="AI39" s="99"/>
@@ -35855,9 +35820,7 @@
       <c r="AC40" s="103"/>
       <c r="AD40" s="102"/>
       <c r="AE40" s="55"/>
-      <c r="AF40" s="102" t="s">
-        <v>701</v>
-      </c>
+      <c r="AF40" s="102"/>
       <c r="AG40" s="173"/>
       <c r="AH40" s="96"/>
       <c r="AI40" s="99"/>
@@ -36923,9 +36886,7 @@
       <c r="AC41" s="103"/>
       <c r="AD41" s="102"/>
       <c r="AE41" s="55"/>
-      <c r="AF41" s="102" t="s">
-        <v>701</v>
-      </c>
+      <c r="AF41" s="102"/>
       <c r="AG41" s="173"/>
       <c r="AH41" s="96"/>
       <c r="AI41" s="99"/>
@@ -37991,9 +37952,7 @@
       <c r="AC42" s="103"/>
       <c r="AD42" s="102"/>
       <c r="AE42" s="55"/>
-      <c r="AF42" s="102" t="s">
-        <v>701</v>
-      </c>
+      <c r="AF42" s="102"/>
       <c r="AG42" s="173"/>
       <c r="AH42" s="96"/>
       <c r="AI42" s="99"/>
@@ -39059,9 +39018,7 @@
       <c r="AC43" s="103"/>
       <c r="AD43" s="102"/>
       <c r="AE43" s="55"/>
-      <c r="AF43" s="102" t="s">
-        <v>701</v>
-      </c>
+      <c r="AF43" s="102"/>
       <c r="AG43" s="173"/>
       <c r="AH43" s="96"/>
       <c r="AI43" s="99"/>
@@ -40127,9 +40084,7 @@
       <c r="AC44" s="103"/>
       <c r="AD44" s="102"/>
       <c r="AE44" s="55"/>
-      <c r="AF44" s="102" t="s">
-        <v>701</v>
-      </c>
+      <c r="AF44" s="102"/>
       <c r="AG44" s="173"/>
       <c r="AH44" s="96"/>
       <c r="AI44" s="99"/>
@@ -41195,9 +41150,7 @@
       <c r="AC45" s="103"/>
       <c r="AD45" s="102"/>
       <c r="AE45" s="55"/>
-      <c r="AF45" s="102" t="s">
-        <v>701</v>
-      </c>
+      <c r="AF45" s="102"/>
       <c r="AG45" s="173"/>
       <c r="AH45" s="96"/>
       <c r="AI45" s="99"/>
@@ -42263,9 +42216,7 @@
       <c r="AC46" s="103"/>
       <c r="AD46" s="102"/>
       <c r="AE46" s="55"/>
-      <c r="AF46" s="102" t="s">
-        <v>701</v>
-      </c>
+      <c r="AF46" s="102"/>
       <c r="AG46" s="173"/>
       <c r="AH46" s="96"/>
       <c r="AI46" s="99"/>
@@ -43331,9 +43282,7 @@
       <c r="AC47" s="103"/>
       <c r="AD47" s="102"/>
       <c r="AE47" s="55"/>
-      <c r="AF47" s="102" t="s">
-        <v>701</v>
-      </c>
+      <c r="AF47" s="102"/>
       <c r="AG47" s="173"/>
       <c r="AH47" s="96"/>
       <c r="AI47" s="99"/>
@@ -44399,9 +44348,7 @@
       <c r="AC48" s="103"/>
       <c r="AD48" s="102"/>
       <c r="AE48" s="55"/>
-      <c r="AF48" s="102" t="s">
-        <v>701</v>
-      </c>
+      <c r="AF48" s="102"/>
       <c r="AG48" s="173"/>
       <c r="AH48" s="96"/>
       <c r="AI48" s="99"/>
@@ -45467,9 +45414,7 @@
       <c r="AC49" s="103"/>
       <c r="AD49" s="102"/>
       <c r="AE49" s="55"/>
-      <c r="AF49" s="102" t="s">
-        <v>701</v>
-      </c>
+      <c r="AF49" s="102"/>
       <c r="AG49" s="173"/>
       <c r="AH49" s="96"/>
       <c r="AI49" s="99"/>
@@ -46535,9 +46480,7 @@
       <c r="AC50" s="103"/>
       <c r="AD50" s="102"/>
       <c r="AE50" s="55"/>
-      <c r="AF50" s="102" t="s">
-        <v>701</v>
-      </c>
+      <c r="AF50" s="102"/>
       <c r="AG50" s="173"/>
       <c r="AH50" s="96"/>
       <c r="AI50" s="99"/>
@@ -46613,9 +46556,7 @@
       <c r="AC51" s="103"/>
       <c r="AD51" s="102"/>
       <c r="AE51" s="55"/>
-      <c r="AF51" s="102" t="s">
-        <v>701</v>
-      </c>
+      <c r="AF51" s="102"/>
       <c r="AG51" s="173"/>
       <c r="AH51" s="96"/>
       <c r="AI51" s="99"/>
@@ -47681,9 +47622,7 @@
       <c r="AC52" s="103"/>
       <c r="AD52" s="102"/>
       <c r="AE52" s="55"/>
-      <c r="AF52" s="102" t="s">
-        <v>701</v>
-      </c>
+      <c r="AF52" s="102"/>
       <c r="AG52" s="173"/>
       <c r="AH52" s="96"/>
       <c r="AI52" s="99"/>
@@ -48749,9 +48688,7 @@
       <c r="AC53" s="103"/>
       <c r="AD53" s="102"/>
       <c r="AE53" s="55"/>
-      <c r="AF53" s="102" t="s">
-        <v>701</v>
-      </c>
+      <c r="AF53" s="102"/>
       <c r="AG53" s="173"/>
       <c r="AH53" s="96"/>
       <c r="AI53" s="99"/>
@@ -49817,9 +49754,7 @@
       <c r="AC54" s="103"/>
       <c r="AD54" s="102"/>
       <c r="AE54" s="55"/>
-      <c r="AF54" s="102" t="s">
-        <v>701</v>
-      </c>
+      <c r="AF54" s="102"/>
       <c r="AG54" s="173"/>
       <c r="AH54" s="96"/>
       <c r="AI54" s="99"/>
@@ -50885,9 +50820,7 @@
       <c r="AC55" s="103"/>
       <c r="AD55" s="102"/>
       <c r="AE55" s="55"/>
-      <c r="AF55" s="102" t="s">
-        <v>701</v>
-      </c>
+      <c r="AF55" s="102"/>
       <c r="AG55" s="173"/>
       <c r="AH55" s="96"/>
       <c r="AI55" s="99"/>
@@ -51953,9 +51886,7 @@
       <c r="AC56" s="103"/>
       <c r="AD56" s="102"/>
       <c r="AE56" s="55"/>
-      <c r="AF56" s="102" t="s">
-        <v>701</v>
-      </c>
+      <c r="AF56" s="102"/>
       <c r="AG56" s="173"/>
       <c r="AH56" s="96"/>
       <c r="AI56" s="99"/>
@@ -72457,7 +72388,7 @@
   <drawing r:id="rId2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="22">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="20">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000004000000}">
           <x14:formula1>
             <xm:f>'Drop down lists'!$E$3:$E$5</xm:f>
@@ -72500,12 +72431,6 @@
           </x14:formula1>
           <xm:sqref>AK15:AK395</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{3537F57E-BB5D-7D49-8715-24A5F9258908}">
-          <x14:formula1>
-            <xm:f>'Drop down lists'!$F$3:$F$203</xm:f>
-          </x14:formula1>
-          <xm:sqref>B395</xm:sqref>
-        </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{A198A72C-F977-B448-940D-6C736E9211D7}">
           <x14:formula1>
             <xm:f>'Drop down lists'!$I$3:$I$7</xm:f>
@@ -72542,12 +72467,6 @@
           </x14:formula1>
           <xm:sqref>AI15:AI394</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{A7CF1B78-A6BE-5F4D-8ECA-CE067F34AEBE}">
-          <x14:formula1>
-            <xm:f>'Drop down lists'!$F$3:$F$205</xm:f>
-          </x14:formula1>
-          <xm:sqref>B15:B394</xm:sqref>
-        </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{4C459A59-671B-2646-953F-0ABF3B6CC601}">
           <x14:formula1>
             <xm:f>'Drop down lists'!$D$3:$D$54</xm:f>
@@ -72570,25 +72489,25 @@
           <x14:formula1>
             <xm:f>'Drop down lists'!$C$4:$C$8</xm:f>
           </x14:formula1>
-          <xm:sqref>D395:E395</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{E7BA82AC-35CB-2742-9F9D-840BD5371448}">
-          <x14:formula1>
-            <xm:f>'Drop down lists'!$C$4:$C$9</xm:f>
-          </x14:formula1>
-          <xm:sqref>D57:D394</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{A09FD080-2305-E347-BC2D-E97E32CA1CFD}">
-          <x14:formula1>
-            <xm:f>'Drop down lists'!$C$3:$C$8</xm:f>
-          </x14:formula1>
-          <xm:sqref>D15:D56</xm:sqref>
+          <xm:sqref>E395</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{B7F70FA2-3EC9-0F43-9634-73E411B71982}">
           <x14:formula1>
             <xm:f>'Drop down lists'!$S$3:$S$5</xm:f>
           </x14:formula1>
           <xm:sqref>AF15:AF394</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{259CF6F3-A3AD-CB41-AD42-1DBDCBFEB0D6}">
+          <x14:formula1>
+            <xm:f>'Drop down lists'!$C$3:$C$9</xm:f>
+          </x14:formula1>
+          <xm:sqref>D15:D1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{5279B6C3-7A02-0A4A-8236-EF72DDA1162F}">
+          <x14:formula1>
+            <xm:f>'Drop down lists'!$F$3:$F$209</xm:f>
+          </x14:formula1>
+          <xm:sqref>B15:B1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -72601,21 +72520,28 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A2:AN205"/>
+  <dimension ref="A2:AN209"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView topLeftCell="A150" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="D202" sqref="D202"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="8.83203125" style="122"/>
-    <col min="2" max="2" width="10.6640625" style="122" customWidth="1"/>
+    <col min="2" max="2" width="11.83203125" style="122" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="24.6640625" style="122" customWidth="1"/>
-    <col min="4" max="4" width="21.1640625" style="122" customWidth="1"/>
-    <col min="5" max="9" width="8.83203125" style="122"/>
+    <col min="4" max="4" width="50" style="122" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="8.83203125" style="122"/>
+    <col min="7" max="7" width="20.5" style="122" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.83203125" style="122"/>
+    <col min="9" max="9" width="10.5" style="122" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="8.83203125" style="35"/>
-    <col min="11" max="16384" width="8.83203125" style="122"/>
+    <col min="11" max="11" width="8.83203125" style="122"/>
+    <col min="12" max="12" width="25" style="122" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.83203125" style="122"/>
+    <col min="14" max="14" width="14.83203125" style="122" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="8.83203125" style="122"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:40" ht="36" x14ac:dyDescent="0.15">
@@ -72827,7 +72753,7 @@
       <c r="D5" s="131" t="s">
         <v>119</v>
       </c>
-      <c r="E5" s="188" t="s">
+      <c r="E5" s="177" t="s">
         <v>97</v>
       </c>
       <c r="F5" s="151" t="s">
@@ -72993,7 +72919,9 @@
     <row r="9" spans="1:40" x14ac:dyDescent="0.15">
       <c r="A9"/>
       <c r="B9" s="161"/>
-      <c r="C9" s="161"/>
+      <c r="C9" s="131" t="s">
+        <v>707</v>
+      </c>
       <c r="D9" s="162" t="s">
         <v>483</v>
       </c>
@@ -78139,6 +78067,26 @@
       <c r="R205"/>
       <c r="S205"/>
     </row>
+    <row r="206" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="F206" s="151" t="s">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="207" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="F207" s="151" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="208" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="F208" s="151" t="s">
+        <v>710</v>
+      </c>
+    </row>
+    <row r="209" spans="6:6" x14ac:dyDescent="0.15">
+      <c r="F209" s="151" t="s">
+        <v>711</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="41" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>